<commit_message>
Corrigido geração da curva de convergência
</commit_message>
<xml_diff>
--- a/resultados/Tabelas TCC/minmaxsdtime.xlsx
+++ b/resultados/Tabelas TCC/minmaxsdtime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezio\Google Drive\TCC\[Code] Identificação de Parâmetros\resultados\17-Feb-2021 10_43_16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezio\Google Drive\TCC\[Code] Identificação de Parâmetros\resultados\Tabelas TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79B7A06-4900-4314-B3EF-CD50704F895D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6BC0D1-78A7-408C-9B80-E1030507FA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4590" yWindow="3390" windowWidth="8415" windowHeight="7875" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D RMSE I - teorica" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,15 @@
     <sheet name="2D RMSE I - 1000 -Mitsubishi" sheetId="19" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -900,10 +909,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="A2:F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1211,6 +1220,12 @@
       </c>
       <c r="F15">
         <v>2.1318187200000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="F16">
+        <f>30*SUM(F2:F15)</f>
+        <v>1125.1177851999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>